<commit_message>
[sysan_reqaly_035] Merges UC002 with UC004 in the traceability matrix
</commit_message>
<xml_diff>
--- a/_development-process_/documents/requirements-document/traceability-matrix.xlsx
+++ b/_development-process_/documents/requirements-document/traceability-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8145" windowHeight="10410"/>
+    <workbookView windowWidth="28695" windowHeight="13530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>USE CASES</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>UC003</t>
-  </si>
-  <si>
-    <t>UC004</t>
   </si>
   <si>
     <t>UC005</t>
@@ -120,10 +117,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -166,8 +163,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -175,21 +234,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,106 +279,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,187 +340,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,15 +587,6 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
@@ -611,41 +599,17 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -666,6 +630,39 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -676,17 +673,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -714,157 +700,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -913,7 +910,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -925,13 +922,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1256,10 +1256,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:I27"/>
+  <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -1271,6 +1271,7 @@
     <col min="10" max="10" width="8.85333333333333" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.5"/>
     <row r="2" spans="2:9">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -1295,352 +1296,350 @@
       <c r="F3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="21" t="s">
         <v>5</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="8"/>
       <c r="G4" s="17"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="21"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="7"/>
       <c r="C5" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="18"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="22"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="17"/>
       <c r="F6" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="21"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="7"/>
       <c r="C7" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="18"/>
+      <c r="E7" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="G7" s="18"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="22"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="17"/>
       <c r="F8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="21"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="7"/>
       <c r="C9" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="18"/>
       <c r="F9" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="22"/>
+      <c r="I9" s="23"/>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="17"/>
+      <c r="E10" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="G10" s="17"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="21"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" s="7"/>
       <c r="C11" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="18"/>
       <c r="F11" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="22"/>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="17"/>
+      <c r="E12" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="G12" s="17"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="21"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="7"/>
       <c r="C13" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="18"/>
+      <c r="E13" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="G13" s="18"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="22"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="17"/>
       <c r="F14" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="21"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="7"/>
       <c r="C15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="18"/>
+      <c r="E15" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="G15" s="18"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="22"/>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="7"/>
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="17"/>
       <c r="F16" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="21"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="7"/>
       <c r="C17" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F17" s="10"/>
-      <c r="G17" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="G17" s="18"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="22"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="17"/>
       <c r="F18" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="21"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="7"/>
       <c r="C19" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="18"/>
       <c r="F19" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="22"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="7"/>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="17"/>
+      <c r="E20" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="G20" s="17"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="21"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="7"/>
       <c r="C21" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="18"/>
       <c r="F21" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="22"/>
+      <c r="I21" s="23"/>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="G22" s="17"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="21"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="7"/>
       <c r="C23" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F23" s="10"/>
-      <c r="G23" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="G23" s="18"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="22"/>
+      <c r="I23" s="23"/>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="17"/>
       <c r="F24" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="21"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="7"/>
       <c r="C25" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="10"/>
-      <c r="E25" s="18"/>
+      <c r="E25" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="G25" s="18"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="22"/>
+      <c r="I25" s="23"/>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" s="7"/>
       <c r="C26" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="17"/>
       <c r="F26" s="8"/>
       <c r="G26" s="17"/>
       <c r="H26" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" s="21"/>
+        <v>8</v>
+      </c>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" ht="13.5" spans="2:9">
       <c r="B27" s="11"/>
       <c r="C27" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="19"/>
       <c r="F27" s="13"/>
       <c r="G27" s="19"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="23" t="s">
-        <v>9</v>
+      <c r="I27" s="24" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[sysan_hlucse_036] Updates the UseCase Diagram based on the modification of the traceability matrix
</commit_message>
<xml_diff>
--- a/_development-process_/documents/requirements-document/traceability-matrix.xlsx
+++ b/_development-process_/documents/requirements-document/traceability-matrix.xlsx
@@ -28,10 +28,10 @@
     <t>UC003</t>
   </si>
   <si>
+    <t>UC004</t>
+  </si>
+  <si>
     <t>UC005</t>
-  </si>
-  <si>
-    <t>UC006</t>
   </si>
   <si>
     <t>FUNCTIONAL REQUIREMENTS</t>
@@ -117,9 +117,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -163,34 +163,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -202,16 +186,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,14 +224,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -240,30 +255,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,7 +279,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,15 +293,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,19 +346,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +478,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,114 +514,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -497,30 +521,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,17 +614,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,20 +647,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -677,17 +677,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,168 +711,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -904,37 +904,34 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1256,23 +1253,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:I27"/>
+  <dimension ref="B2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9.8" customWidth="1"/>
     <col min="2" max="2" width="1.7" customWidth="1"/>
     <col min="3" max="3" width="6.2" customWidth="1"/>
-    <col min="4" max="9" width="6.4" customWidth="1"/>
-    <col min="10" max="10" width="8.85333333333333" customWidth="1"/>
+    <col min="4" max="8" width="6.4" customWidth="1"/>
+    <col min="9" max="9" width="8.85333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5"/>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:8">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
@@ -1281,30 +1277,28 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="2:9">
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="H3" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:8">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1314,337 +1308,313 @@
       <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="22"/>
-    </row>
-    <row r="5" spans="2:9">
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5" s="7"/>
       <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="2:8">
       <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="17"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="2:8">
       <c r="B7" s="7"/>
       <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="2:9">
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="2:8">
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="17"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="22"/>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="2:8">
       <c r="B9" s="7"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="18"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="2:9">
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="2:8">
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="22"/>
-    </row>
-    <row r="11" spans="2:9">
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="2:8">
       <c r="B11" s="7"/>
       <c r="C11" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="18"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="2:8">
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="2:8">
       <c r="B13" s="7"/>
       <c r="C13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="2:9">
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="2:8">
       <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="G14" s="18"/>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="2:8">
       <c r="B15" s="7"/>
       <c r="C15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="2:9">
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="2:8">
       <c r="B16" s="7"/>
       <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="17"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="2:8">
       <c r="B17" s="7"/>
       <c r="C17" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="10"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="2:8">
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="17"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="22"/>
-    </row>
-    <row r="19" spans="2:9">
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="2:8">
       <c r="B19" s="7"/>
       <c r="C19" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="2:8">
       <c r="B20" s="7"/>
       <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="22"/>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="2:8">
       <c r="B21" s="7"/>
       <c r="C21" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="10"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="23"/>
-    </row>
-    <row r="22" spans="2:9">
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="2:8">
       <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="22"/>
-    </row>
-    <row r="23" spans="2:9">
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="2:8">
       <c r="B23" s="7"/>
       <c r="C23" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="10"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="23"/>
-    </row>
-    <row r="24" spans="2:9">
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="2:8">
       <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="17"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="22"/>
-    </row>
-    <row r="25" spans="2:9">
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="2:8">
       <c r="B25" s="7"/>
       <c r="C25" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="10"/>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="23"/>
-    </row>
-    <row r="26" spans="2:9">
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="2:8">
       <c r="B26" s="7"/>
       <c r="C26" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="8"/>
-      <c r="E26" s="17"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" s="22"/>
-    </row>
-    <row r="27" ht="13.5" spans="2:9">
+      <c r="G26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" ht="13.5" spans="2:8">
       <c r="B27" s="11"/>
       <c r="C27" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="19"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="24" t="s">
+      <c r="G27" s="22"/>
+      <c r="H27" s="23" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D2:H2"/>
     <mergeCell ref="B4:B27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>